<commit_message>
Fixed conference pie chart picture
</commit_message>
<xml_diff>
--- a/NFL2018/Weekly Forecasts/WeekCon.xlsx
+++ b/NFL2018/Weekly Forecasts/WeekCon.xlsx
@@ -624,11 +624,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9986945749760489</v>
+        <v>0.9986493672078596</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.9866135241172136</v>
+        <v>0.9867409286714661</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -637,11 +637,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>94.26995306113889</v>
+        <v>94.26568575630718</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>91.2492731432214</v>
+        <v>91.26105645318675</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -650,16 +650,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.5212670957465808</v>
+        <v>0.5216320956735808</v>
       </c>
       <c r="C6" s="8">
-        <v>0.4787329042534191</v>
+        <v>0.4783679043264191</v>
       </c>
       <c r="E6" s="8">
-        <v>0.5680075863984827</v>
+        <v>0.5676841864631627</v>
       </c>
       <c r="F6" s="8">
-        <v>0.4319924136015173</v>
+        <v>0.4323158135368373</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -667,16 +667,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>31.40311671937665</v>
+        <v>31.4199085160183</v>
       </c>
       <c r="C7" s="9">
-        <v>30.33959953208009</v>
+        <v>30.34254753149049</v>
       </c>
       <c r="E7" s="9">
-        <v>33.30626893874621</v>
+        <v>33.29916054016789</v>
       </c>
       <c r="F7" s="9">
-        <v>29.89195042160992</v>
+        <v>29.88830682233863</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -990,7 +990,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="10">
         <v>55</v>

</xml_diff>